<commit_message>
New versions of plots (horizontal) Also, new DLS/Zeta data in folders
</commit_message>
<xml_diff>
--- a/CCK8-Transfection_Plots/20240202_CCK8-Transfection_DIPLibrary_PBS.xlsx
+++ b/CCK8-Transfection_Plots/20240202_CCK8-Transfection_DIPLibrary_PBS.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/aryellewright/Documents/Documents - Aryelle’s MacBook Air/Kumar-Biomaterials-Lab/CCK8_Transfection_Plots/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/aryellewright/Documents/Documents - Aryelle’s MacBook Air/Kumar-Biomaterials-Lab/CCK8-Transfection_Plots/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FBEDB065-B024-5949-B4E9-310E47BDE5F3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6CAF4590-742B-D640-93E0-F2F4BC95020D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3180" yWindow="1380" windowWidth="20980" windowHeight="15260" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="9780" yWindow="1300" windowWidth="20980" windowHeight="15260" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Plate 1 - Sheet1" sheetId="1" r:id="rId1"/>
@@ -3698,8 +3698,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EA1AD3B1-023C-284E-8C37-00F9307BF6C3}">
   <dimension ref="A1:H11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D7" sqref="D7:E11"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C25" sqref="C25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -4343,8 +4343,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1E612818-6CDE-494B-962E-466FBDDAC96C}">
   <dimension ref="A1:E15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G21" sqref="G21"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:E15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>

</xml_diff>